<commit_message>
TSLA, updated LNW, Hedgefund BTC Holdings from Hedgefollow, KVYO
</commit_message>
<xml_diff>
--- a/Gaming/IGT.xlsx
+++ b/Gaming/IGT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Documents\models\Gaming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BEB8FFD-0542-4886-83C2-31A5D0088796}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7B28FE0-064D-41DE-84A5-6D20D10FF8E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -595,9 +595,6 @@
     <t>Inventories</t>
   </si>
   <si>
-    <t>Interest Rate debt</t>
-  </si>
-  <si>
     <t>RG1</t>
   </si>
   <si>
@@ -917,6 +914,9 @@
   </si>
   <si>
     <t>D&amp;A</t>
+  </si>
+  <si>
+    <t>Debt y/y</t>
   </si>
 </sst>
 </file>
@@ -1827,6 +1827,10 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="7" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1884,10 +1888,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="7" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -22072,7 +22072,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:N46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
@@ -22094,7 +22094,7 @@
   <sheetData>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2" s="34" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C2" s="19"/>
       <c r="E2" s="24" t="s">
@@ -22131,23 +22131,23 @@
         <v>45369</v>
       </c>
       <c r="E3" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="F3" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="F3" s="28" t="s">
-        <v>107</v>
-      </c>
       <c r="H3" t="s">
+        <v>125</v>
+      </c>
+      <c r="I3" s="10" t="s">
         <v>126</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>127</v>
       </c>
       <c r="J3" s="39"/>
       <c r="L3" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="M3" t="s">
         <v>128</v>
-      </c>
-      <c r="M3" t="s">
-        <v>129</v>
       </c>
       <c r="N3" s="38"/>
     </row>
@@ -22157,18 +22157,18 @@
         <v>0.71736111111111112</v>
       </c>
       <c r="E4" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="F4" s="28" t="s">
         <v>108</v>
-      </c>
-      <c r="F4" s="28" t="s">
-        <v>109</v>
       </c>
       <c r="I4" s="10"/>
       <c r="J4" s="39"/>
       <c r="L4" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="M4" t="s">
         <v>130</v>
-      </c>
-      <c r="M4" t="s">
-        <v>131</v>
       </c>
       <c r="N4" s="13"/>
     </row>
@@ -22176,18 +22176,18 @@
       <c r="B5" s="5"/>
       <c r="C5" s="13"/>
       <c r="E5" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="F5" s="28" t="s">
         <v>110</v>
-      </c>
-      <c r="F5" s="28" t="s">
-        <v>111</v>
       </c>
       <c r="I5" s="10"/>
       <c r="J5" s="39"/>
       <c r="L5" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="M5" t="s">
         <v>132</v>
-      </c>
-      <c r="M5" t="s">
-        <v>133</v>
       </c>
       <c r="N5" s="13"/>
     </row>
@@ -22199,18 +22199,18 @@
         <v>20.34</v>
       </c>
       <c r="E6" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="F6" s="28" t="s">
         <v>112</v>
-      </c>
-      <c r="F6" s="28" t="s">
-        <v>113</v>
       </c>
       <c r="I6" s="10"/>
       <c r="J6" s="39"/>
       <c r="L6" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="M6" t="s">
         <v>134</v>
-      </c>
-      <c r="M6" t="s">
-        <v>135</v>
       </c>
       <c r="N6" s="13"/>
     </row>
@@ -22223,18 +22223,18 @@
         <v>200</v>
       </c>
       <c r="E7" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F7" s="28" t="s">
         <v>114</v>
-      </c>
-      <c r="F7" s="28" t="s">
-        <v>115</v>
       </c>
       <c r="I7" s="10"/>
       <c r="J7" s="39"/>
       <c r="L7" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="M7" t="s">
         <v>136</v>
-      </c>
-      <c r="M7" t="s">
-        <v>137</v>
       </c>
       <c r="N7" s="13"/>
     </row>
@@ -22247,18 +22247,18 @@
         <v>4068</v>
       </c>
       <c r="E8" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="F8" s="28" t="s">
         <v>116</v>
-      </c>
-      <c r="F8" s="28" t="s">
-        <v>117</v>
       </c>
       <c r="I8" s="10"/>
       <c r="J8" s="39"/>
       <c r="L8" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="M8" t="s">
         <v>138</v>
-      </c>
-      <c r="M8" t="s">
-        <v>139</v>
       </c>
       <c r="N8" s="13"/>
     </row>
@@ -22271,18 +22271,18 @@
         <v>572</v>
       </c>
       <c r="E9" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="F9" s="28" t="s">
         <v>118</v>
-      </c>
-      <c r="F9" s="28" t="s">
-        <v>119</v>
       </c>
       <c r="I9" s="10"/>
       <c r="J9" s="39"/>
       <c r="L9" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="M9" t="s">
         <v>140</v>
-      </c>
-      <c r="M9" t="s">
-        <v>141</v>
       </c>
       <c r="N9" s="13"/>
     </row>
@@ -22295,18 +22295,18 @@
         <v>5671</v>
       </c>
       <c r="E10" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="F10" s="28" t="s">
         <v>120</v>
-      </c>
-      <c r="F10" s="28" t="s">
-        <v>121</v>
       </c>
       <c r="I10" s="10"/>
       <c r="J10" s="39"/>
       <c r="L10" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="M10" t="s">
         <v>142</v>
-      </c>
-      <c r="M10" t="s">
-        <v>143</v>
       </c>
       <c r="N10" s="13"/>
     </row>
@@ -22319,18 +22319,18 @@
         <v>-5099</v>
       </c>
       <c r="E11" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="F11" s="28" t="s">
         <v>122</v>
-      </c>
-      <c r="F11" s="28" t="s">
-        <v>123</v>
       </c>
       <c r="I11" s="10"/>
       <c r="J11" s="39"/>
       <c r="L11" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="M11" t="s">
         <v>144</v>
-      </c>
-      <c r="M11" t="s">
-        <v>145</v>
       </c>
       <c r="N11" s="13"/>
     </row>
@@ -22343,17 +22343,17 @@
         <v>9167</v>
       </c>
       <c r="E12" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="F12" s="28" t="s">
         <v>124</v>
-      </c>
-      <c r="F12" s="28" t="s">
-        <v>125</v>
       </c>
       <c r="J12" s="13"/>
       <c r="L12" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="M12" t="s">
         <v>146</v>
-      </c>
-      <c r="M12" t="s">
-        <v>147</v>
       </c>
       <c r="N12" s="13"/>
     </row>
@@ -22417,11 +22417,11 @@
       <c r="E17" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="L17" s="129" t="s">
-        <v>148</v>
-      </c>
-      <c r="M17" s="130"/>
-      <c r="N17" s="131"/>
+      <c r="L17" s="133" t="s">
+        <v>147</v>
+      </c>
+      <c r="M17" s="134"/>
+      <c r="N17" s="135"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
@@ -22432,11 +22432,11 @@
         <v>0.12021005081874646</v>
       </c>
       <c r="E18" t="s">
-        <v>149</v>
-      </c>
-      <c r="L18" s="132"/>
-      <c r="M18" s="133"/>
-      <c r="N18" s="134"/>
+        <v>148</v>
+      </c>
+      <c r="L18" s="136"/>
+      <c r="M18" s="137"/>
+      <c r="N18" s="138"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
@@ -22446,45 +22446,45 @@
         <f>C15/(C17*100)</f>
         <v>0.31040189573459726</v>
       </c>
-      <c r="L19" s="132"/>
-      <c r="M19" s="133"/>
-      <c r="N19" s="134"/>
+      <c r="L19" s="136"/>
+      <c r="M19" s="137"/>
+      <c r="N19" s="138"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C20" s="6">
         <f>Model!G6/Model!F5-1</f>
         <v>1.3921113689095099E-2</v>
       </c>
-      <c r="L20" s="132"/>
-      <c r="M20" s="133"/>
-      <c r="N20" s="134"/>
+      <c r="L20" s="136"/>
+      <c r="M20" s="137"/>
+      <c r="N20" s="138"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C21" s="6">
         <f>Model!H6/Model!G6-1</f>
         <v>3.6613272311212919E-2</v>
       </c>
-      <c r="L21" s="132"/>
-      <c r="M21" s="133"/>
-      <c r="N21" s="134"/>
+      <c r="L21" s="136"/>
+      <c r="M21" s="137"/>
+      <c r="N21" s="138"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C22" s="148">
+      <c r="C22" s="129">
         <f>Model!F18+Model!F11</f>
         <v>864</v>
       </c>
-      <c r="L22" s="132"/>
-      <c r="M22" s="133"/>
-      <c r="N22" s="134"/>
+      <c r="L22" s="136"/>
+      <c r="M22" s="137"/>
+      <c r="N22" s="138"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
@@ -22494,9 +22494,9 @@
         <f>Model!F18</f>
         <v>630</v>
       </c>
-      <c r="L23" s="132"/>
-      <c r="M23" s="133"/>
-      <c r="N23" s="134"/>
+      <c r="L23" s="136"/>
+      <c r="M23" s="137"/>
+      <c r="N23" s="138"/>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
@@ -22506,9 +22506,9 @@
         <f>Model!F25</f>
         <v>0.48886310904872388</v>
       </c>
-      <c r="L24" s="132"/>
-      <c r="M24" s="133"/>
-      <c r="N24" s="134"/>
+      <c r="L24" s="136"/>
+      <c r="M24" s="137"/>
+      <c r="N24" s="138"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
@@ -22518,9 +22518,9 @@
         <f>Model!F26</f>
         <v>7.1461716937354994E-2</v>
       </c>
-      <c r="L25" s="132"/>
-      <c r="M25" s="133"/>
-      <c r="N25" s="134"/>
+      <c r="L25" s="136"/>
+      <c r="M25" s="137"/>
+      <c r="N25" s="138"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
@@ -22530,40 +22530,40 @@
         <f>C12/C23</f>
         <v>14.550793650793651</v>
       </c>
-      <c r="L26" s="132"/>
-      <c r="M26" s="133"/>
-      <c r="N26" s="134"/>
+      <c r="L26" s="136"/>
+      <c r="M26" s="137"/>
+      <c r="N26" s="138"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B27" s="149" t="s">
-        <v>95</v>
-      </c>
-      <c r="C27" s="150">
+      <c r="B27" s="130" t="s">
+        <v>94</v>
+      </c>
+      <c r="C27" s="131">
         <f>(Model!F52+Model!F56)/Model!F61</f>
         <v>2.9052254098360657</v>
       </c>
       <c r="E27" t="s">
         <v>82</v>
       </c>
-      <c r="L27" s="132"/>
-      <c r="M27" s="133"/>
-      <c r="N27" s="134"/>
+      <c r="L27" s="136"/>
+      <c r="M27" s="137"/>
+      <c r="N27" s="138"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C28" s="36">
         <f>C22/-Model!F15</f>
         <v>3.0315789473684212</v>
       </c>
-      <c r="L28" s="135"/>
-      <c r="M28" s="136"/>
-      <c r="N28" s="137"/>
+      <c r="L28" s="139"/>
+      <c r="M28" s="140"/>
+      <c r="N28" s="141"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C29" s="36">
         <f>Model!F42/Model!F55</f>
@@ -22572,7 +22572,7 @@
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C30" s="36">
         <f>(Model!F37+Model!F39+Model!F38)/Model!F55</f>
@@ -22580,17 +22580,17 @@
       </c>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B31" s="149" t="s">
-        <v>99</v>
-      </c>
-      <c r="C31" s="151">
+      <c r="B31" s="130" t="s">
+        <v>98</v>
+      </c>
+      <c r="C31" s="132">
         <f>(Model!F42-Model!F55)/Model!F49</f>
         <v>4.1180966940569462E-2</v>
       </c>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C32" s="50">
         <f>(Model!F49-Model!F60)/C7</f>
@@ -22599,7 +22599,7 @@
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C33" s="36">
         <f>Model!F5/Model!F49</f>
@@ -22608,7 +22608,7 @@
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C34" s="39">
         <f>Model!F20/Model!F49</f>
@@ -22617,7 +22617,7 @@
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C35" s="39">
         <f>Model!F20/Model!F61</f>
@@ -22626,7 +22626,7 @@
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" s="22" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C36" s="23"/>
     </row>
@@ -22685,11 +22685,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7345E9-1C5F-45F5-BD7C-66FA029FFFF4}">
   <dimension ref="A1:X82"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B36" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomRight" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22997,7 +22997,7 @@
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B10" s="10">
         <v>850</v>
@@ -23031,7 +23031,7 @@
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B11" s="10">
         <v>266</v>
@@ -23065,7 +23065,7 @@
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B12" s="10">
         <v>25</v>
@@ -23251,7 +23251,7 @@
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B16" s="10">
         <v>40</v>
@@ -23517,7 +23517,7 @@
     </row>
     <row r="21" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B21" s="10">
         <f>-126-5</f>
@@ -24042,7 +24042,7 @@
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B31" s="3"/>
       <c r="C31" s="40"/>
@@ -24492,7 +24492,7 @@
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B43" s="10"/>
       <c r="C43" s="10">
@@ -24775,7 +24775,7 @@
     </row>
     <row r="51" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B51" s="10"/>
       <c r="C51" s="10">
@@ -24805,7 +24805,7 @@
     </row>
     <row r="52" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B52" s="10"/>
       <c r="C52" s="10">
@@ -24835,7 +24835,7 @@
     </row>
     <row r="53" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B53" s="10"/>
       <c r="C53" s="10">
@@ -25181,13 +25181,22 @@
     </row>
     <row r="63" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>92</v>
+        <v>199</v>
       </c>
       <c r="B63" s="58"/>
       <c r="C63" s="58"/>
-      <c r="D63" s="58"/>
-      <c r="E63" s="58"/>
-      <c r="F63" s="59"/>
+      <c r="D63" s="58">
+        <f>D56/C56-1</f>
+        <v>-0.17563955708285606</v>
+      </c>
+      <c r="E63" s="58">
+        <f t="shared" ref="E63:F63" si="17">E56/D56-1</f>
+        <v>-0.12150687046472131</v>
+      </c>
+      <c r="F63" s="59">
+        <f t="shared" si="17"/>
+        <v>-6.1511423550087985E-3</v>
+      </c>
       <c r="V63" s="16"/>
     </row>
     <row r="81" spans="6:22" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -40677,16 +40686,16 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H1" s="142" t="s">
         <v>159</v>
       </c>
-      <c r="H1" s="138" t="s">
-        <v>160</v>
-      </c>
-      <c r="I1" s="139"/>
-      <c r="J1" s="139"/>
-      <c r="K1" s="139"/>
-      <c r="L1" s="139"/>
-      <c r="M1" s="140"/>
+      <c r="I1" s="143"/>
+      <c r="J1" s="143"/>
+      <c r="K1" s="143"/>
+      <c r="L1" s="143"/>
+      <c r="M1" s="144"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="12">
@@ -40718,22 +40727,22 @@
         <v>-5.0502159247454381E-2</v>
       </c>
       <c r="H3" s="70" t="s">
+        <v>160</v>
+      </c>
+      <c r="I3" s="71" t="s">
         <v>161</v>
       </c>
-      <c r="I3" s="71" t="s">
+      <c r="J3" s="72" t="s">
         <v>162</v>
       </c>
-      <c r="J3" s="72" t="s">
+      <c r="K3" s="73" t="s">
         <v>163</v>
       </c>
-      <c r="K3" s="73" t="s">
+      <c r="L3" s="73" t="s">
         <v>164</v>
       </c>
-      <c r="L3" s="73" t="s">
+      <c r="M3" s="74" t="s">
         <v>165</v>
-      </c>
-      <c r="M3" s="74" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -41145,7 +41154,7 @@
       </c>
       <c r="H15" s="86"/>
       <c r="I15" s="87" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J15" s="87">
         <f>COUNTIF(D:D,"&gt;"&amp;H14)</f>
@@ -41189,10 +41198,10 @@
         <f t="shared" si="0"/>
         <v>-5.4426616599467792E-3</v>
       </c>
-      <c r="H17" s="141" t="s">
-        <v>168</v>
-      </c>
-      <c r="I17" s="142"/>
+      <c r="H17" s="145" t="s">
+        <v>167</v>
+      </c>
+      <c r="I17" s="146"/>
       <c r="M17" s="90"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
@@ -41206,8 +41215,8 @@
         <f t="shared" si="0"/>
         <v>5.1057217810668298E-3</v>
       </c>
-      <c r="H18" s="143"/>
-      <c r="I18" s="144"/>
+      <c r="H18" s="147"/>
+      <c r="I18" s="148"/>
       <c r="M18" s="90"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
@@ -41222,7 +41231,7 @@
         <v>1.5555582305992077E-2</v>
       </c>
       <c r="H19" s="91" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I19" s="92">
         <f>AVERAGE(D:D)</f>
@@ -41242,7 +41251,7 @@
         <v>-1.4245717679850722E-2</v>
       </c>
       <c r="H20" s="91" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I20" s="92">
         <f>_xlfn.STDEV.S(D:D)/SQRT(COUNT(D:D))</f>
@@ -41262,7 +41271,7 @@
         <v>1.582623900043667E-2</v>
       </c>
       <c r="H21" s="91" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I21" s="92">
         <f>MEDIAN(D:D)</f>
@@ -41282,7 +41291,7 @@
         <v>1.2672361739856086E-2</v>
       </c>
       <c r="H22" s="91" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I22" s="92">
         <f>MODE(D:D)</f>
@@ -41302,7 +41311,7 @@
         <v>-5.9281056512642261E-3</v>
       </c>
       <c r="H23" s="91" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I23" s="92">
         <f>_xlfn.STDEV.S(D:D)</f>
@@ -41322,7 +41331,7 @@
         <v>-4.2907818735959391E-2</v>
       </c>
       <c r="H24" s="91" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I24" s="92">
         <f>_xlfn.VAR.S(D:D)</f>
@@ -41342,7 +41351,7 @@
         <v>4.5606300205593087E-2</v>
       </c>
       <c r="H25" s="91" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I25" s="93">
         <f>KURT(D:D)</f>
@@ -41362,7 +41371,7 @@
         <v>-9.2224849293361055E-2</v>
       </c>
       <c r="H26" s="91" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I26" s="93">
         <f>SKEW(D:D)</f>
@@ -41382,7 +41391,7 @@
         <v>-2.8450001418557136E-2</v>
       </c>
       <c r="H27" s="91" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I27" s="92">
         <f>I29-I28</f>
@@ -41402,7 +41411,7 @@
         <v>-7.1428422825750015E-3</v>
       </c>
       <c r="H28" s="91" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I28" s="92">
         <f>MIN(D:D)</f>
@@ -41422,7 +41431,7 @@
         <v>1.5831125890573894E-2</v>
       </c>
       <c r="H29" s="91" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I29" s="92">
         <f>MAX(D:D)</f>
@@ -41442,7 +41451,7 @@
         <v>-1.972197981195456E-2</v>
       </c>
       <c r="H30" s="91" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I30" s="93">
         <f>SUM(D:D)</f>
@@ -41462,7 +41471,7 @@
         <v>-5.0353008717644587E-2</v>
       </c>
       <c r="H31" s="94" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I31" s="69">
         <f>COUNT(D:D)</f>
@@ -41497,16 +41506,16 @@
       </c>
       <c r="H33" s="96"/>
       <c r="I33" s="97" t="s">
+        <v>180</v>
+      </c>
+      <c r="J33" s="97" t="s">
+        <v>179</v>
+      </c>
+      <c r="K33" s="97" t="s">
         <v>181</v>
       </c>
-      <c r="J33" s="97" t="s">
-        <v>180</v>
-      </c>
-      <c r="K33" s="97" t="s">
+      <c r="L33" s="98" t="s">
         <v>182</v>
-      </c>
-      <c r="L33" s="98" t="s">
-        <v>183</v>
       </c>
       <c r="M33" s="90"/>
     </row>
@@ -41522,7 +41531,7 @@
         <v>3.2423733461737658E-2</v>
       </c>
       <c r="H34" s="99" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I34" s="84">
         <f>AVERAGEIF(D:D,"&gt;0")</f>
@@ -41554,7 +41563,7 @@
         <v>1.212600985225909E-2</v>
       </c>
       <c r="H35" s="99" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I35" s="84">
         <f>AVERAGEIF(D:D,"&lt;0")</f>
@@ -41586,7 +41595,7 @@
         <v>-3.3998813698273289E-2</v>
       </c>
       <c r="H36" s="100" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I36" s="87">
         <v>0</v>
@@ -41635,22 +41644,22 @@
         <v>-2.8981268692158779E-2</v>
       </c>
       <c r="H38" s="75" t="s">
+        <v>186</v>
+      </c>
+      <c r="I38" s="97" t="s">
         <v>187</v>
       </c>
-      <c r="I38" s="97" t="s">
+      <c r="J38" s="97" t="s">
         <v>188</v>
       </c>
-      <c r="J38" s="97" t="s">
+      <c r="K38" s="97" t="s">
         <v>189</v>
       </c>
-      <c r="K38" s="97" t="s">
+      <c r="L38" s="97" t="s">
         <v>190</v>
       </c>
-      <c r="L38" s="97" t="s">
+      <c r="M38" s="98" t="s">
         <v>191</v>
-      </c>
-      <c r="M38" s="98" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.25">
@@ -41780,14 +41789,14 @@
         <f t="shared" si="0"/>
         <v>4.9358213096166947E-2</v>
       </c>
-      <c r="H43" s="145" t="s">
-        <v>193</v>
-      </c>
-      <c r="I43" s="146"/>
-      <c r="J43" s="146"/>
-      <c r="K43" s="146"/>
-      <c r="L43" s="146"/>
-      <c r="M43" s="147"/>
+      <c r="H43" s="149" t="s">
+        <v>192</v>
+      </c>
+      <c r="I43" s="150"/>
+      <c r="J43" s="150"/>
+      <c r="K43" s="150"/>
+      <c r="L43" s="150"/>
+      <c r="M43" s="151"/>
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B44" s="12">
@@ -42298,7 +42307,7 @@
         <v>6.6666750993839896E-2</v>
       </c>
       <c r="H60" s="119" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I60" s="120"/>
     </row>
@@ -42314,7 +42323,7 @@
         <v>-4.1353393899412394E-2</v>
       </c>
       <c r="H61" s="121" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I61" s="122"/>
     </row>
@@ -42343,7 +42352,7 @@
         <v>-2.7255969711705852E-2</v>
       </c>
       <c r="H63" s="119" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I63" s="124"/>
     </row>
@@ -42359,7 +42368,7 @@
         <v>1.8379569177671806E-2</v>
       </c>
       <c r="H64" s="125" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I64" s="126">
         <f>I63*(1-I60)</f>
@@ -42378,7 +42387,7 @@
         <v>6.6826668996072813E-2</v>
       </c>
       <c r="H65" s="121" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I65" s="127">
         <f>I63*(1+I61)</f>

</xml_diff>